<commit_message>
created proto heat maps for longo data
</commit_message>
<xml_diff>
--- a/To_Share/001_Fit_Assay_Extinction_Summary.xlsx
+++ b/To_Share/001_Fit_Assay_Extinction_Summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boterolab1/Box Sync/CB_VF_Shared/Wet_Lab/Projects/FS/FS_Analysis/3_Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boterolab1/Box Sync/CB_VF_Shared/Wet_Lab/Projects/FS/FS_Analysis/To_Share/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D360E8EB-E4D9-DC4D-A5E0-B1AC1116C468}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7325323C-775E-3540-BC33-D7F8D577362F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="-15540" windowWidth="23840" windowHeight="13840" xr2:uid="{B49486D9-2F4B-CB4B-962B-6442749A8107}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{B49486D9-2F4B-CB4B-962B-6442749A8107}"/>
   </bookViews>
   <sheets>
     <sheet name="00&amp;80" sheetId="1" r:id="rId1"/>
@@ -563,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3729E91C-17DE-6242-91E7-F70206A6E2C2}">
   <dimension ref="A2:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>